<commit_message>
Intro a Semantica 1
+ Creación clases semantica y matrizSemantica
</commit_message>
<xml_diff>
--- a/Producciones.xlsx
+++ b/Producciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\Documents\NetBeansProjects\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C632E1-B5C9-4AD2-8078-B383802C17BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D55AD-95A1-406F-89CA-F64DCE0D6FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2E2150B-4EBC-493D-997F-5AEA11C60ED9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2E2150B-4EBC-493D-997F-5AEA11C60ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -5458,9 +5458,6 @@
     </r>
   </si>
   <si>
-    <t>(876-877)</t>
-  </si>
-  <si>
     <t>(812 - 816)</t>
   </si>
   <si>
@@ -5868,6 +5865,9 @@
       </rPr>
       <t>@</t>
     </r>
+  </si>
+  <si>
+    <t>(820-821)</t>
   </si>
 </sst>
 </file>
@@ -6425,6 +6425,9 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="16" borderId="12" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6447,9 +6450,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6907,8 +6907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3FA8B9-A47E-429A-BD32-FD36D0235D3B}">
   <dimension ref="B1:DI168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6933,40 +6933,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
-      <c r="J1" s="58" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+      <c r="J1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58" t="s">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="2:113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="Q2" s="65" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="Q2" s="66" t="s">
         <v>333</v>
       </c>
-      <c r="R2" s="65"/>
+      <c r="R2" s="66"/>
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
@@ -7077,7 +7077,7 @@
         <v>330</v>
       </c>
       <c r="F3" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G3" s="44" t="s">
         <v>331</v>
@@ -7128,7 +7128,7 @@
         <v>345</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G4" s="48" t="s">
         <v>336</v>
@@ -7173,10 +7173,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G5" s="46" t="s">
         <v>339</v>
@@ -7224,7 +7224,7 @@
         <v>342</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" s="47" t="s">
         <v>340</v>
@@ -7272,7 +7272,7 @@
         <v>343</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G7" s="43" t="s">
         <v>341</v>
@@ -7862,7 +7862,7 @@
         <v>350</v>
       </c>
       <c r="F22" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G22" s="50" t="s">
         <v>347</v>
@@ -7910,7 +7910,7 @@
         <v>351</v>
       </c>
       <c r="F23" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G23" s="51" t="s">
         <v>346</v>
@@ -7958,13 +7958,13 @@
         <v>352</v>
       </c>
       <c r="F24" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G24" s="52" t="s">
         <v>348</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>167</v>
@@ -8006,13 +8006,13 @@
         <v>353</v>
       </c>
       <c r="F25" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G25" s="53" t="s">
         <v>349</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>168</v>
@@ -8090,7 +8090,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="1"/>
@@ -8177,13 +8177,13 @@
         <v>27</v>
       </c>
       <c r="F29" s="55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G29" s="54" t="s">
-        <v>369</v>
-      </c>
-      <c r="H29" s="66">
-        <v>820</v>
+        <v>368</v>
+      </c>
+      <c r="H29" s="58">
+        <v>850</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="9" t="s">
@@ -8223,7 +8223,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="1"/>
@@ -8264,7 +8264,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="1"/>
@@ -8305,7 +8305,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>175</v>
@@ -8344,7 +8344,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>176</v>
@@ -8495,7 +8495,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J37" s="9" t="s">
         <v>211</v>
@@ -8530,7 +8530,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>180</v>
@@ -8550,10 +8550,10 @@
       <c r="O38" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="Q38" s="65" t="s">
+      <c r="Q38" s="66" t="s">
         <v>332</v>
       </c>
-      <c r="R38" s="65"/>
+      <c r="R38" s="66"/>
       <c r="S38" s="37"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
@@ -9123,7 +9123,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
@@ -9269,16 +9269,16 @@
         <v>1</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F71" s="55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G71" s="57" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H71" s="45">
-        <v>821</v>
+        <v>851</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
@@ -9379,13 +9379,13 @@
         <v>357</v>
       </c>
       <c r="F78" s="55" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G78" s="56" t="s">
         <v>356</v>
       </c>
       <c r="H78" s="45" t="s">
-        <v>358</v>
+        <v>374</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
S2: 1010, 1020 e Interfaz
</commit_message>
<xml_diff>
--- a/Producciones.xlsx
+++ b/Producciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\Documents\NetBeansProjects\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A93E72C-B026-4902-8029-DB8B7A8AE2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EFCC7F-6CF0-4421-A0E5-496480545531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13755" yWindow="2205" windowWidth="14250" windowHeight="13260" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
+    <workbookView xWindow="13380" yWindow="1935" windowWidth="14430" windowHeight="11385" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="419">
   <si>
     <t>PRODUCIONES</t>
   </si>
@@ -6346,6 +6346,285 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF7A7E6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EST A3</t>
+    </r>
+  </si>
+  <si>
+    <t>End EST</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>ID debe ser clase procedimiento</t>
+  </si>
+  <si>
+    <t>ID debe ser clase funcion</t>
+  </si>
+  <si>
+    <t>ID debe ser declarado antes de ser utilizado</t>
+  </si>
+  <si>
+    <t>A, s1</t>
+  </si>
+  <si>
+    <t>Se esperaba rango positivo</t>
+  </si>
+  <si>
+    <t>For value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">@ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFA401"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFA401"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EST A3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">End </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <t>863 , 864</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">def </t>
     </r>
     <r>
@@ -6470,6 +6749,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">@ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD3034D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>@</t>
     </r>
     <r>
@@ -6495,290 +6784,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF7A7E6"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EST A3</t>
-    </r>
-  </si>
-  <si>
-    <t>End EST</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>ID debe ser clase procedimiento</t>
-  </si>
-  <si>
-    <t>ID debe ser clase funcion</t>
-  </si>
-  <si>
-    <t>ID debe ser declarado antes de ser utilizado</t>
-  </si>
-  <si>
-    <t>A, s1</t>
-  </si>
-  <si>
-    <t>Se esperaba rango positivo</t>
-  </si>
-  <si>
-    <t>For value</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">@ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFA401"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFA401"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> EST A3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">End </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-  </si>
-  <si>
-    <t>863 , 864</t>
+    <t>No return?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7076,8 +7089,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD3034D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7209,6 +7229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3034D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7374,7 +7400,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7542,6 +7568,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis5" xfId="6" builtinId="46"/>
@@ -7677,6 +7704,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD3034D"/>
       <color rgb="FFF7A7E6"/>
       <color rgb="FF9999FF"/>
       <color rgb="FFA50021"/>
@@ -7686,7 +7714,6 @@
       <color rgb="FFCC0000"/>
       <color rgb="FFF3E529"/>
       <color rgb="FFE0AAB9"/>
-      <color rgb="FFFFA605"/>
     </mruColors>
   </colors>
   <extLst>
@@ -7999,8 +8026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3FA8B9-A47E-429A-BD32-FD36D0235D3B}">
   <dimension ref="B1:DI168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8217,7 +8244,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>334</v>
@@ -8409,16 +8436,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F8" s="54" t="s">
-        <v>409</v>
-      </c>
-      <c r="G8" s="74" t="s">
         <v>408</v>
       </c>
+      <c r="G8" s="87" t="s">
+        <v>418</v>
+      </c>
       <c r="H8" s="45">
-        <v>862</v>
+        <v>1150</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>127</v>
@@ -8459,7 +8486,15 @@
       <c r="E9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="45"/>
+      <c r="F9" s="54" t="s">
+        <v>408</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>407</v>
+      </c>
+      <c r="H9" s="45">
+        <v>862</v>
+      </c>
       <c r="J9" s="9" t="s">
         <v>128</v>
       </c>
@@ -9058,7 +9093,7 @@
         <v>319</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G24" s="52" t="s">
         <v>315</v>
@@ -10428,7 +10463,7 @@
         <v>775</v>
       </c>
       <c r="R63" s="42" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.25">
@@ -10469,7 +10504,7 @@
         <v>776</v>
       </c>
       <c r="R64" s="42" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
@@ -10492,7 +10527,7 @@
         <v>777</v>
       </c>
       <c r="R65" s="42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
@@ -10525,7 +10560,7 @@
         <v>778</v>
       </c>
       <c r="R66" s="76" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
@@ -10548,7 +10583,7 @@
         <v>779</v>
       </c>
       <c r="R67" s="76" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
@@ -10725,10 +10760,10 @@
         <v>364</v>
       </c>
       <c r="J77" s="77" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K77" s="45" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
@@ -10742,7 +10777,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F78" s="54" t="s">
         <v>334</v>

</xml_diff>

<commit_message>
S2: 1030, 1040, 1050 parcialmente arregladas
</commit_message>
<xml_diff>
--- a/Producciones.xlsx
+++ b/Producciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\Documents\NetBeansProjects\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EFCC7F-6CF0-4421-A0E5-496480545531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E086F-353D-4876-A5C4-C41AA6A84A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="1935" windowWidth="14430" windowHeight="11385" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="14430" windowHeight="11385" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="422">
   <si>
     <t>PRODUCIONES</t>
   </si>
@@ -4728,9 +4728,6 @@
     </r>
   </si>
   <si>
-    <t>(820-821)</t>
-  </si>
-  <si>
     <t>Incompatibilidad de tipos …</t>
   </si>
   <si>
@@ -5674,6 +5671,857 @@
     <t>S2</t>
   </si>
   <si>
+    <t>IF (booleano)</t>
+  </si>
+  <si>
+    <t>ERRORES DE SEMANTICA 1</t>
+  </si>
+  <si>
+    <t>ELIF (booleano)</t>
+  </si>
+  <si>
+    <t>WHILE (booleano)</t>
+  </si>
+  <si>
+    <t>La EXP tiene que ser Booleana</t>
+  </si>
+  <si>
+    <t>ID debe ser mismo tipo que EXP</t>
+  </si>
+  <si>
+    <t>La cant. de dimensiones utilizadas en una lista de arreglo debe ser igual a la declarada</t>
+  </si>
+  <si>
+    <t>1010 - 1012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1020 - 1021</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I0</t>
+    </r>
+  </si>
+  <si>
+    <t>(822 - 824)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">OR I1 I2 </t>
+  </si>
+  <si>
+    <t>Lista-Arreglo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ARR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">@ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA50021"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> J2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>860 - 861</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">J0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">J1 </t>
+    </r>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>La organizacion de los datos de inicializacion de una lista tipo arr deben tener un orden</t>
+  </si>
+  <si>
+    <t>Fuera de limite</t>
+  </si>
+  <si>
+    <t>Los diccionarios no tienen posiciones negativas</t>
+  </si>
+  <si>
+    <t>Diferente valor de llave</t>
+  </si>
+  <si>
+    <t>Las tuplas no tienen posiciones negativas</t>
+  </si>
+  <si>
+    <t>Fuera de dimension</t>
+  </si>
+  <si>
+    <t>La EXP debe ser entera</t>
+  </si>
+  <si>
+    <t>ERRORES DE SEMANTICA 2</t>
+  </si>
+  <si>
+    <t>845 - 846</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> J5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <t>ID debe ser var, par, arr, list, dicc, rang para recibir valor</t>
+  </si>
+  <si>
+    <t>La cant. de parametros debe ser igual a la declarada</t>
+  </si>
+  <si>
+    <t>Valor invalido</t>
+  </si>
+  <si>
+    <t>Id for</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">OR  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA50021"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <r>
+      <t>Return</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9999FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <t>(804, -804)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF7A7E6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EST A3</t>
+    </r>
+  </si>
+  <si>
+    <t>End EST</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>ID debe ser clase procedimiento</t>
+  </si>
+  <si>
+    <t>ID debe ser clase funcion</t>
+  </si>
+  <si>
+    <t>ID debe ser declarado antes de ser utilizado</t>
+  </si>
+  <si>
+    <t>A, s1</t>
+  </si>
+  <si>
+    <t>Se esperaba rango positivo</t>
+  </si>
+  <si>
+    <t>For value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">@ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFA401"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFA401"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EST A3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">End </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+  </si>
+  <si>
+    <t>863 , 864</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">def </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> id ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PROGRAM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">@ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD3034D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A0</t>
+    </r>
+  </si>
+  <si>
+    <t>No return?</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -5693,6 +6541,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> OR </t>
     </r>
     <r>
@@ -5761,10 +6630,129 @@
     </r>
   </si>
   <si>
-    <t>IF (booleano)</t>
-  </si>
-  <si>
-    <t>ERRORES DE SEMANTICA 1</t>
+    <t>(820, 821)</t>
+  </si>
+  <si>
+    <t>1009, 1010</t>
+  </si>
+  <si>
+    <r>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF7A7E6"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26AD5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">OR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26AD5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wend</t>
+    </r>
   </si>
   <si>
     <r>
@@ -5786,6 +6774,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> OR </t>
     </r>
     <r>
@@ -5853,945 +6862,17 @@
     </r>
   </si>
   <si>
-    <t>ELIF (booleano)</t>
-  </si>
-  <si>
-    <t>WHILE (booleano)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">while </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">OR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF26AD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EST</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>wend</t>
-    </r>
-  </si>
-  <si>
-    <t>La EXP tiene que ser Booleana</t>
-  </si>
-  <si>
-    <t>ID debe ser mismo tipo que EXP</t>
-  </si>
-  <si>
-    <t>La cant. de dimensiones utilizadas en una lista de arreglo debe ser igual a la declarada</t>
-  </si>
-  <si>
-    <t>1010 - 1012</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1020 - 1021</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I0</t>
-    </r>
-  </si>
-  <si>
-    <t>(822 - 824)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I0</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">OR I1 I2 </t>
-  </si>
-  <si>
-    <t>Lista-Arreglo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ARR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">@ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFA50021"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>860 - 861</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">J0 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">J1 </t>
-    </r>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>La organizacion de los datos de inicializacion de una lista tipo arr deben tener un orden</t>
-  </si>
-  <si>
-    <t>Fuera de limite</t>
-  </si>
-  <si>
-    <t>Los diccionarios no tienen posiciones negativas</t>
-  </si>
-  <si>
-    <t>Diferente valor de llave</t>
-  </si>
-  <si>
-    <t>Las tuplas no tienen posiciones negativas</t>
-  </si>
-  <si>
-    <t>Fuera de dimension</t>
-  </si>
-  <si>
-    <t>La EXP debe ser entera</t>
-  </si>
-  <si>
-    <t>ERRORES DE SEMANTICA 2</t>
-  </si>
-  <si>
-    <t>845 - 846</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> J5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-  </si>
-  <si>
-    <t>ID debe ser var, par, arr, list, dicc, rang para recibir valor</t>
-  </si>
-  <si>
-    <t>La cant. de parametros debe ser igual a la declarada</t>
-  </si>
-  <si>
-    <t>Valor invalido</t>
-  </si>
-  <si>
-    <t>Id for</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">OR  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFA50021"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <r>
-      <t>Return</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9999FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-  </si>
-  <si>
-    <t>(804, -804)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFF7A7E6"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EST A3</t>
-    </r>
-  </si>
-  <si>
-    <t>End EST</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>ID debe ser clase procedimiento</t>
-  </si>
-  <si>
-    <t>ID debe ser clase funcion</t>
-  </si>
-  <si>
-    <t>ID debe ser declarado antes de ser utilizado</t>
-  </si>
-  <si>
-    <t>A, s1</t>
-  </si>
-  <si>
-    <t>Se esperaba rango positivo</t>
-  </si>
-  <si>
-    <t>For value</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">@ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFA401"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFA401"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> EST A3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">End </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-  </si>
-  <si>
-    <t>863 , 864</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">def </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> id ( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="7"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">PROGRAM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">@ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD3034D"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A0</t>
-    </r>
-  </si>
-  <si>
-    <t>No return?</t>
+    <t>1009, 1012</t>
+  </si>
+  <si>
+    <t>1009, 1011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7092,6 +7173,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFD3034D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -7400,7 +7488,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7541,6 +7629,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7568,7 +7657,9 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis5" xfId="6" builtinId="46"/>
@@ -7704,12 +7795,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF26AD5"/>
+      <color rgb="FFF7A7E6"/>
       <color rgb="FFD3034D"/>
-      <color rgb="FFF7A7E6"/>
       <color rgb="FF9999FF"/>
       <color rgb="FFA50021"/>
       <color rgb="FF0099CC"/>
-      <color rgb="FFF26AD5"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFCC0000"/>
       <color rgb="FFF3E529"/>
@@ -8026,8 +8117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3FA8B9-A47E-429A-BD32-FD36D0235D3B}">
   <dimension ref="B1:DI168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8052,40 +8143,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="82"/>
-      <c r="J1" s="79" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
+      <c r="J1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79" t="s">
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="2:113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="Q2" s="86" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="Q2" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="R2" s="86"/>
+      <c r="R2" s="87"/>
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
@@ -8244,7 +8335,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>334</v>
@@ -8301,7 +8392,7 @@
         <v>307</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>124</v>
@@ -8436,13 +8527,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F8" s="54" t="s">
-        <v>408</v>
-      </c>
-      <c r="G8" s="87" t="s">
-        <v>418</v>
+        <v>404</v>
+      </c>
+      <c r="G8" s="78" t="s">
+        <v>414</v>
       </c>
       <c r="H8" s="45">
         <v>1150</v>
@@ -8487,10 +8578,10 @@
         <v>68</v>
       </c>
       <c r="F9" s="54" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="H9" s="45">
         <v>862</v>
@@ -9093,7 +9184,7 @@
         <v>319</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="G24" s="52" t="s">
         <v>315</v>
@@ -9557,7 +9648,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J35" s="38" t="s">
         <v>153</v>
@@ -9685,10 +9776,10 @@
       <c r="O38" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="Q38" s="86" t="s">
+      <c r="Q38" s="87" t="s">
         <v>300</v>
       </c>
-      <c r="R38" s="86"/>
+      <c r="R38" s="87"/>
       <c r="S38" s="37"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
@@ -9741,7 +9832,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>157</v>
@@ -9811,7 +9902,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>159</v>
@@ -9863,10 +9954,10 @@
       <c r="O43" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="Q43" s="78" t="s">
-        <v>367</v>
-      </c>
-      <c r="R43" s="78"/>
+      <c r="Q43" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="R43" s="79"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" s="34">
@@ -9879,7 +9970,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>161</v>
@@ -9903,7 +9994,7 @@
         <v>750</v>
       </c>
       <c r="R44" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
@@ -9917,7 +10008,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>162</v>
@@ -9983,7 +10074,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>164</v>
@@ -10003,10 +10094,10 @@
       <c r="O47" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="Q47" s="78" t="s">
-        <v>394</v>
-      </c>
-      <c r="R47" s="78"/>
+      <c r="Q47" s="79" t="s">
+        <v>390</v>
+      </c>
+      <c r="R47" s="79"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B48" s="34">
@@ -10019,16 +10110,16 @@
         <v>1</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>334</v>
       </c>
       <c r="G48" s="51" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="H48" s="45" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>165</v>
@@ -10049,13 +10140,13 @@
         <v>291</v>
       </c>
       <c r="P48" s="68" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="Q48" s="62">
         <v>760</v>
       </c>
       <c r="R48" s="16" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10069,7 +10160,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>166</v>
@@ -10090,13 +10181,13 @@
         <v>291</v>
       </c>
       <c r="P49" s="69" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="Q49" s="62">
         <v>761</v>
       </c>
       <c r="R49" s="67" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
@@ -10110,7 +10201,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J50" s="9" t="s">
         <v>167</v>
@@ -10137,7 +10228,7 @@
         <v>762</v>
       </c>
       <c r="R50" s="16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
@@ -10178,7 +10269,7 @@
         <v>763</v>
       </c>
       <c r="R51" s="16" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
@@ -10201,7 +10292,7 @@
         <v>764</v>
       </c>
       <c r="R52" s="42" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
@@ -10224,7 +10315,7 @@
         <v>765</v>
       </c>
       <c r="R53" s="42" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
@@ -10247,7 +10338,7 @@
         <v>766</v>
       </c>
       <c r="R54" s="42" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
@@ -10270,7 +10361,7 @@
         <v>767</v>
       </c>
       <c r="R55" s="42" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
@@ -10293,7 +10384,7 @@
         <v>768</v>
       </c>
       <c r="R56" s="61" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
@@ -10316,7 +10407,7 @@
         <v>769</v>
       </c>
       <c r="R57" s="42" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.25">
@@ -10339,7 +10430,7 @@
         <v>770</v>
       </c>
       <c r="R58" s="42" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
@@ -10362,7 +10453,7 @@
         <v>771</v>
       </c>
       <c r="R59" s="42" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
@@ -10385,7 +10476,7 @@
         <v>772</v>
       </c>
       <c r="R60" s="42" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
@@ -10399,13 +10490,13 @@
         <v>1</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>335</v>
       </c>
       <c r="G61" s="70" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="H61" s="45">
         <v>844</v>
@@ -10417,7 +10508,7 @@
         <v>773</v>
       </c>
       <c r="R61" s="42" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
@@ -10440,7 +10531,7 @@
         <v>774</v>
       </c>
       <c r="R62" s="42" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.25">
@@ -10463,7 +10554,7 @@
         <v>775</v>
       </c>
       <c r="R63" s="42" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.25">
@@ -10477,16 +10568,16 @@
         <v>1</v>
       </c>
       <c r="E64" s="31" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F64" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G64" s="51" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="I64" s="54" t="s">
         <v>335</v>
@@ -10504,7 +10595,7 @@
         <v>776</v>
       </c>
       <c r="R64" s="42" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
@@ -10518,7 +10609,7 @@
         <v>1</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P65" s="71">
         <v>1130</v>
@@ -10527,7 +10618,7 @@
         <v>777</v>
       </c>
       <c r="R65" s="42" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
@@ -10541,16 +10632,16 @@
         <v>1</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F66" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G66" s="72" t="s">
         <v>307</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I66" s="2"/>
       <c r="P66" s="71">
@@ -10560,7 +10651,7 @@
         <v>778</v>
       </c>
       <c r="R66" s="76" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
@@ -10583,7 +10674,7 @@
         <v>779</v>
       </c>
       <c r="R67" s="76" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
@@ -10644,7 +10735,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F71" s="54" t="s">
         <v>335</v>
@@ -10653,7 +10744,7 @@
         <v>328</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I71" s="54"/>
       <c r="K71" s="45"/>
@@ -10745,25 +10836,25 @@
         <v>1</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>365</v>
+        <v>415</v>
       </c>
       <c r="F77" s="54" t="s">
+        <v>363</v>
+      </c>
+      <c r="G77" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="G77" s="47" t="s">
-        <v>366</v>
-      </c>
-      <c r="H77" s="45">
-        <v>1010</v>
+      <c r="H77" s="88" t="s">
+        <v>417</v>
       </c>
       <c r="I77" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J77" s="77" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="K77" s="45" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
@@ -10777,7 +10868,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F78" s="54" t="s">
         <v>334</v>
@@ -10786,7 +10877,7 @@
         <v>323</v>
       </c>
       <c r="H78" s="45" t="s">
-        <v>338</v>
+        <v>416</v>
       </c>
       <c r="I78" s="54" t="s">
         <v>334</v>
@@ -10809,16 +10900,16 @@
         <v>1</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>371</v>
+        <v>418</v>
       </c>
       <c r="F79" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G79" s="65" t="s">
-        <v>370</v>
-      </c>
-      <c r="H79" s="45">
-        <v>1011</v>
+        <v>367</v>
+      </c>
+      <c r="H79" s="88" t="s">
+        <v>421</v>
       </c>
       <c r="I79" s="54" t="s">
         <v>334</v>
@@ -10871,13 +10962,13 @@
         <v>1</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F82" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G82" s="73" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="H82" s="45">
         <v>1140</v>
@@ -10924,16 +11015,16 @@
         <v>1</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>368</v>
+        <v>419</v>
       </c>
       <c r="F85" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G85" s="63" t="s">
-        <v>369</v>
-      </c>
-      <c r="H85" s="45">
-        <v>1012</v>
+        <v>366</v>
+      </c>
+      <c r="H85" s="88" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
@@ -10977,7 +11068,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H88" s="45"/>
     </row>
@@ -10992,7 +11083,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
@@ -11006,7 +11097,7 @@
         <v>1</v>
       </c>
       <c r="E90" s="31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -11020,7 +11111,7 @@
         <v>1</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
@@ -11034,7 +11125,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
@@ -11048,7 +11139,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -11062,7 +11153,7 @@
         <v>1</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
@@ -11076,7 +11167,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -11090,7 +11181,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
@@ -11104,7 +11195,7 @@
         <v>1</v>
       </c>
       <c r="E97" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
@@ -11132,7 +11223,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
@@ -11160,7 +11251,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
@@ -11188,7 +11279,7 @@
         <v>1</v>
       </c>
       <c r="E103" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
@@ -11216,7 +11307,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
@@ -11230,7 +11321,7 @@
         <v>1</v>
       </c>
       <c r="E106" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
@@ -11524,13 +11615,13 @@
         <v>1</v>
       </c>
       <c r="E127" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F127" s="54" t="s">
         <v>335</v>
       </c>
       <c r="G127" s="58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H127" s="45">
         <v>853</v>

</xml_diff>

<commit_message>
Sem3: reglas de entrada
</commit_message>
<xml_diff>
--- a/Producciones.xlsx
+++ b/Producciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\Documents\NetBeansProjects\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A9EFAA-B3FC-4389-9AAE-D88CBC7304D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CACAA87-C920-40D8-BC7F-6A3EB4ADAC30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="0" windowWidth="22620" windowHeight="15600" activeTab="2" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
+    <workbookView xWindow="1560" yWindow="45" windowWidth="15630" windowHeight="15600" activeTab="2" xr2:uid="{CE99D781-93EC-43B9-9325-D9E8261D5F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Producciones" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="442">
   <si>
     <t>PRODUCIONES</t>
   </si>
@@ -7136,6 +7136,33 @@
   </si>
   <si>
     <t>Paramertro debe ser tipo cadena, id, idlista o  idcadena</t>
+  </si>
+  <si>
+    <t>Numero de parametros incorrecto</t>
+  </si>
+  <si>
+    <t>Parametro debe ser tipo idlista, idcadena, iddicc, idtup, o idrang</t>
+  </si>
+  <si>
+    <t>Parametro debe ser tipo decimal o id</t>
+  </si>
+  <si>
+    <t>Parametro debe ser tipo idlista</t>
+  </si>
+  <si>
+    <t>Parametro debe ser tipo idlista num</t>
+  </si>
+  <si>
+    <t>Parametro debe ser tipo decimal, float, hex, oct, bin, complejo, cadena o char</t>
+  </si>
+  <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>Salidas</t>
+  </si>
+  <si>
+    <t>Uso</t>
   </si>
 </sst>
 </file>
@@ -7623,7 +7650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -7826,6 +7853,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -7836,7 +7876,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7969,33 +8009,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8056,6 +8069,45 @@
     <xf numFmtId="0" fontId="33" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis5" xfId="6" builtinId="46"/>
@@ -8599,34 +8651,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="76"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="106"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="2:113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="77"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
       <c r="V2" s="18"/>
@@ -8761,22 +8813,22 @@
       <c r="E4" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="77" t="s">
         <v>312</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="H4" s="88" t="s">
+      <c r="H4" s="79" t="s">
         <v>378</v>
       </c>
-      <c r="I4" s="90" t="s">
+      <c r="I4" s="81" t="s">
         <v>312</v>
       </c>
-      <c r="J4" s="91" t="s">
+      <c r="J4" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="75" t="s">
         <v>285</v>
       </c>
     </row>
@@ -8802,13 +8854,13 @@
       <c r="H5" s="44">
         <v>805</v>
       </c>
-      <c r="I5" s="85" t="s">
+      <c r="I5" s="76" t="s">
         <v>312</v>
       </c>
-      <c r="J5" s="92" t="s">
+      <c r="J5" s="83" t="s">
         <v>402</v>
       </c>
-      <c r="K5" s="93" t="s">
+      <c r="K5" s="84" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8834,13 +8886,13 @@
       <c r="H6" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="I6" s="94" t="s">
+      <c r="I6" s="85" t="s">
         <v>381</v>
       </c>
-      <c r="J6" s="95" t="s">
+      <c r="J6" s="86" t="s">
         <v>391</v>
       </c>
-      <c r="K6" s="96">
+      <c r="K6" s="87">
         <v>1150</v>
       </c>
     </row>
@@ -9034,7 +9086,7 @@
       <c r="E19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="81"/>
+      <c r="L19" s="72"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="33">
@@ -9172,13 +9224,13 @@
       <c r="F26" s="51" t="s">
         <v>404</v>
       </c>
-      <c r="G26" s="109" t="s">
+      <c r="G26" s="100" t="s">
         <v>407</v>
       </c>
       <c r="H26" s="44">
         <v>871</v>
       </c>
-      <c r="O26" s="81"/>
+      <c r="O26" s="72"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="33">
@@ -9253,7 +9305,7 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="1"/>
-      <c r="L30" s="81"/>
+      <c r="L30" s="72"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="33">
@@ -9284,7 +9336,7 @@
       <c r="E32" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="L32" s="81"/>
+      <c r="L32" s="72"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="33">
@@ -9313,7 +9365,7 @@
       <c r="E34" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="81"/>
+      <c r="L34" s="72"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="33">
@@ -9370,8 +9422,8 @@
       <c r="E38" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="Q38" s="83"/>
-      <c r="R38" s="83"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="74"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="33">
@@ -9442,8 +9494,8 @@
       <c r="E43" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="Q43" s="83"/>
-      <c r="R43" s="83"/>
+      <c r="Q43" s="74"/>
+      <c r="R43" s="74"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="33">
@@ -9500,8 +9552,8 @@
       <c r="E47" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="Q47" s="83"/>
-      <c r="R47" s="83"/>
+      <c r="Q47" s="74"/>
+      <c r="R47" s="74"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="33">
@@ -9758,22 +9810,22 @@
       <c r="E64" s="31" t="s">
         <v>357</v>
       </c>
-      <c r="F64" s="86" t="s">
+      <c r="F64" s="77" t="s">
         <v>341</v>
       </c>
-      <c r="G64" s="97" t="s">
+      <c r="G64" s="88" t="s">
         <v>356</v>
       </c>
-      <c r="H64" s="88" t="s">
+      <c r="H64" s="79" t="s">
         <v>358</v>
       </c>
-      <c r="I64" s="98" t="s">
+      <c r="I64" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="J64" s="99" t="s">
+      <c r="J64" s="90" t="s">
         <v>399</v>
       </c>
-      <c r="K64" s="100">
+      <c r="K64" s="91">
         <v>851</v>
       </c>
     </row>
@@ -9865,10 +9917,10 @@
       <c r="E69" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="F69" s="89" t="s">
+      <c r="F69" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G69" s="111" t="s">
+      <c r="G69" s="102" t="s">
         <v>411</v>
       </c>
       <c r="H69" s="10">
@@ -9959,16 +10011,16 @@
       <c r="D74" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E74" s="102" t="s">
+      <c r="E74" s="93" t="s">
         <v>403</v>
       </c>
-      <c r="F74" s="86" t="s">
+      <c r="F74" s="77" t="s">
         <v>404</v>
       </c>
-      <c r="G74" s="110" t="s">
+      <c r="G74" s="101" t="s">
         <v>406</v>
       </c>
-      <c r="H74" s="100">
+      <c r="H74" s="91">
         <v>870</v>
       </c>
     </row>
@@ -10038,22 +10090,22 @@
       <c r="E78" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="F78" s="86" t="s">
+      <c r="F78" s="77" t="s">
         <v>312</v>
       </c>
-      <c r="G78" s="101" t="s">
+      <c r="G78" s="92" t="s">
         <v>302</v>
       </c>
-      <c r="H78" s="88" t="s">
+      <c r="H78" s="79" t="s">
         <v>393</v>
       </c>
-      <c r="I78" s="90" t="s">
+      <c r="I78" s="81" t="s">
         <v>341</v>
       </c>
-      <c r="J78" s="106" t="s">
+      <c r="J78" s="97" t="s">
         <v>387</v>
       </c>
-      <c r="K78" s="103" t="s">
+      <c r="K78" s="94" t="s">
         <v>389</v>
       </c>
     </row>
@@ -10079,13 +10131,13 @@
       <c r="H79" s="71" t="s">
         <v>398</v>
       </c>
-      <c r="I79" s="85" t="s">
+      <c r="I79" s="76" t="s">
         <v>312</v>
       </c>
-      <c r="J79" s="105" t="s">
+      <c r="J79" s="96" t="s">
         <v>278</v>
       </c>
-      <c r="K79" s="93" t="s">
+      <c r="K79" s="84" t="s">
         <v>284</v>
       </c>
     </row>
@@ -10103,13 +10155,13 @@
         <v>71</v>
       </c>
       <c r="H80" s="44"/>
-      <c r="I80" s="94" t="s">
+      <c r="I80" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="J80" s="104" t="s">
+      <c r="J80" s="95" t="s">
         <v>283</v>
       </c>
-      <c r="K80" s="96" t="s">
+      <c r="K80" s="87" t="s">
         <v>285</v>
       </c>
     </row>
@@ -10522,10 +10574,10 @@
       <c r="E107" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="F107" s="89" t="s">
+      <c r="F107" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G107" s="112" t="s">
+      <c r="G107" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H107" s="10">
@@ -10545,10 +10597,10 @@
       <c r="E108" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="F108" s="89" t="s">
+      <c r="F108" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G108" s="112" t="s">
+      <c r="G108" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H108" s="10">
@@ -10568,10 +10620,10 @@
       <c r="E109" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="F109" s="89" t="s">
+      <c r="F109" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G109" s="112" t="s">
+      <c r="G109" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H109" s="10">
@@ -10591,10 +10643,10 @@
       <c r="E110" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="F110" s="89" t="s">
+      <c r="F110" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G110" s="112" t="s">
+      <c r="G110" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H110" s="10">
@@ -10614,10 +10666,10 @@
       <c r="E111" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="F111" s="89" t="s">
+      <c r="F111" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G111" s="112" t="s">
+      <c r="G111" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H111" s="10">
@@ -10637,10 +10689,10 @@
       <c r="E112" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="F112" s="89" t="s">
+      <c r="F112" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G112" s="112" t="s">
+      <c r="G112" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H112" s="10">
@@ -10660,10 +10712,10 @@
       <c r="E113" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="F113" s="89" t="s">
+      <c r="F113" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G113" s="112" t="s">
+      <c r="G113" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H113" s="10">
@@ -10683,10 +10735,10 @@
       <c r="E114" s="27" t="s">
         <v>421</v>
       </c>
-      <c r="F114" s="89" t="s">
+      <c r="F114" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G114" s="112" t="s">
+      <c r="G114" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H114" s="10">
@@ -10706,10 +10758,10 @@
       <c r="E115" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="F115" s="89" t="s">
+      <c r="F115" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G115" s="112" t="s">
+      <c r="G115" s="103" t="s">
         <v>412</v>
       </c>
       <c r="H115" s="10">
@@ -10729,10 +10781,10 @@
       <c r="E116" s="27" t="s">
         <v>423</v>
       </c>
-      <c r="F116" s="89" t="s">
+      <c r="F116" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G116" s="111" t="s">
+      <c r="G116" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H116" s="10">
@@ -10752,10 +10804,10 @@
       <c r="E117" s="27" t="s">
         <v>424</v>
       </c>
-      <c r="F117" s="89" t="s">
+      <c r="F117" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G117" s="111" t="s">
+      <c r="G117" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H117" s="10">
@@ -10775,10 +10827,10 @@
       <c r="E118" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="F118" s="89" t="s">
+      <c r="F118" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G118" s="111" t="s">
+      <c r="G118" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H118" s="10">
@@ -10798,10 +10850,10 @@
       <c r="E119" s="27" t="s">
         <v>431</v>
       </c>
-      <c r="F119" s="89" t="s">
+      <c r="F119" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G119" s="111" t="s">
+      <c r="G119" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H119" s="10">
@@ -10821,10 +10873,10 @@
       <c r="E120" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="F120" s="89" t="s">
+      <c r="F120" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G120" s="111" t="s">
+      <c r="G120" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H120" s="10">
@@ -10858,10 +10910,10 @@
       <c r="E122" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="F122" s="89" t="s">
+      <c r="F122" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G122" s="111" t="s">
+      <c r="G122" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H122" s="10">
@@ -10881,10 +10933,10 @@
       <c r="E123" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="F123" s="89" t="s">
+      <c r="F123" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G123" s="111" t="s">
+      <c r="G123" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H123" s="10">
@@ -10932,10 +10984,10 @@
       <c r="E126" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="F126" s="89" t="s">
+      <c r="F126" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="G126" s="111" t="s">
+      <c r="G126" s="102" t="s">
         <v>413</v>
       </c>
       <c r="H126" s="10">
@@ -11269,10 +11321,10 @@
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
-      <c r="C153" s="107" t="s">
+      <c r="C153" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="D153" s="108" t="s">
+      <c r="D153" s="99" t="s">
         <v>1</v>
       </c>
       <c r="E153" s="15" t="s">
@@ -11365,16 +11417,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
@@ -11916,16 +11968,16 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="73" t="s">
+      <c r="B57" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="110"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
+      <c r="B58" s="110"/>
+      <c r="C58" s="110"/>
+      <c r="D58" s="110"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
@@ -12477,10 +12529,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F154BECE-C098-4765-AEF8-6AC2AF134C96}">
-  <dimension ref="B4:E74"/>
+  <dimension ref="B4:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12489,10 +12541,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="111" t="s">
         <v>280</v>
       </c>
-      <c r="D4" s="80"/>
+      <c r="D4" s="111"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
@@ -12796,10 +12848,10 @@
       <c r="E39" s="36"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="80" t="s">
+      <c r="C40" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="D40" s="80"/>
+      <c r="D40" s="111"/>
       <c r="E40" s="36"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
@@ -12820,10 +12872,10 @@
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="72" t="s">
+      <c r="C45" s="112" t="s">
         <v>343</v>
       </c>
-      <c r="D45" s="72"/>
+      <c r="D45" s="112"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="58">
@@ -12838,10 +12890,10 @@
       <c r="D47" s="62"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="72" t="s">
+      <c r="C49" s="112" t="s">
         <v>367</v>
       </c>
-      <c r="D49" s="72"/>
+      <c r="D49" s="112"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="64" t="s">
@@ -13008,7 +13060,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="67">
         <v>1110</v>
       </c>
@@ -13019,7 +13071,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="67">
         <v>1120</v>
       </c>
@@ -13030,7 +13082,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="67">
         <v>1130</v>
       </c>
@@ -13041,36 +13093,36 @@
         <v>384</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="67">
         <v>1160</v>
       </c>
-      <c r="C68" s="82">
+      <c r="C68" s="73">
         <v>778</v>
       </c>
       <c r="D68" s="41" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="67">
         <v>1161</v>
       </c>
-      <c r="C69" s="82">
+      <c r="C69" s="73">
         <v>779</v>
       </c>
       <c r="D69" s="41" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="72" t="s">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="112" t="s">
         <v>409</v>
       </c>
-      <c r="D72" s="72"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="64">
+      <c r="D72" s="112"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="113">
         <v>2001</v>
       </c>
       <c r="C73" s="58">
@@ -13079,9 +13131,12 @@
       <c r="D73" s="16" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="64">
+      <c r="E73" s="114" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="113">
         <v>2002</v>
       </c>
       <c r="C74" s="58">
@@ -13090,9 +13145,208 @@
       <c r="D74" s="16" t="s">
         <v>432</v>
       </c>
+      <c r="E74" s="115"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="113">
+        <v>2003</v>
+      </c>
+      <c r="C75" s="58">
+        <v>782</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="E75" s="115"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="113">
+        <v>2004</v>
+      </c>
+      <c r="C76" s="58">
+        <v>783</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="E76" s="115"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="113">
+        <v>2005</v>
+      </c>
+      <c r="C77" s="58">
+        <v>784</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="E77" s="115"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="113">
+        <v>2006</v>
+      </c>
+      <c r="C78" s="58">
+        <v>785</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="E78" s="115"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="113">
+        <v>2007</v>
+      </c>
+      <c r="C79" s="58">
+        <v>786</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="E79" s="116"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="113">
+        <v>2008</v>
+      </c>
+      <c r="C80" s="58">
+        <v>787</v>
+      </c>
+      <c r="D80" s="16"/>
+      <c r="E80" s="114" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="113">
+        <v>2009</v>
+      </c>
+      <c r="C81" s="58">
+        <v>788</v>
+      </c>
+      <c r="D81" s="16"/>
+      <c r="E81" s="115"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="113">
+        <v>2010</v>
+      </c>
+      <c r="C82" s="58">
+        <v>789</v>
+      </c>
+      <c r="D82" s="16"/>
+      <c r="E82" s="115"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="113">
+        <v>2011</v>
+      </c>
+      <c r="C83" s="58">
+        <v>790</v>
+      </c>
+      <c r="D83" s="16"/>
+      <c r="E83" s="115"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="113">
+        <v>2012</v>
+      </c>
+      <c r="C84" s="58">
+        <v>791</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="115"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="113">
+        <v>2013</v>
+      </c>
+      <c r="C85" s="58">
+        <v>792</v>
+      </c>
+      <c r="D85" s="16"/>
+      <c r="E85" s="115"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="113">
+        <v>2014</v>
+      </c>
+      <c r="C86" s="58">
+        <v>793</v>
+      </c>
+      <c r="D86" s="16"/>
+      <c r="E86" s="115"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="113">
+        <v>2015</v>
+      </c>
+      <c r="C87" s="58">
+        <v>794</v>
+      </c>
+      <c r="D87" s="16"/>
+      <c r="E87" s="116"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="113">
+        <v>2016</v>
+      </c>
+      <c r="C88" s="58">
+        <v>795</v>
+      </c>
+      <c r="D88" s="16"/>
+      <c r="E88" s="114" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="113">
+        <v>2017</v>
+      </c>
+      <c r="C89" s="58">
+        <v>796</v>
+      </c>
+      <c r="D89" s="16"/>
+      <c r="E89" s="115"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="113">
+        <v>2018</v>
+      </c>
+      <c r="C90" s="58">
+        <v>797</v>
+      </c>
+      <c r="D90" s="16"/>
+      <c r="E90" s="115"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="113">
+        <v>2019</v>
+      </c>
+      <c r="C91" s="58">
+        <v>798</v>
+      </c>
+      <c r="D91" s="16"/>
+      <c r="E91" s="116"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="113">
+        <v>2020</v>
+      </c>
+      <c r="C92" s="58">
+        <v>799</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>433</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="E73:E79"/>
+    <mergeCell ref="E80:E87"/>
+    <mergeCell ref="E88:E91"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C45:D45"/>

</xml_diff>